<commit_message>
upgrade Upload User function - lms
</commit_message>
<xml_diff>
--- a/lms/lmsfrontend/public/static/excels/sample-upload-user.xlsx
+++ b/lms/lmsfrontend/public/static/excels/sample-upload-user.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiend\OneDrive\Documents\GR\openerp-micro-service\lms\lmsfrontend\public\static\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020EE1B5-3BCB-4C6D-B118-DA67B155FCB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4811B0E0-7A9B-4F99-8CF0-123F80679F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4997FDAE-1009-4185-8539-3E77536A8C0F}"/>
   </bookViews>
@@ -68,6 +68,12 @@
     <t>account</t>
   </si>
   <si>
+    <t>Email*</t>
+  </si>
+  <si>
+    <t>test99.ac@sis.hust.edu.vn</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Note:
 - If </t>
@@ -75,7 +81,7 @@
     <r>
       <rPr>
         <i/>
-        <sz val="11"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -85,7 +91,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -96,7 +102,7 @@
     <r>
       <rPr>
         <i/>
-        <sz val="11"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -106,7 +112,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -118,7 +124,7 @@
     <r>
       <rPr>
         <i/>
-        <sz val="11"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -128,27 +134,41 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>is not provided, the default value will be "password"</t>
-    </r>
-  </si>
-  <si>
-    <t>Email*</t>
-  </si>
-  <si>
-    <t>test99.ac@sis.hust.edu.vn</t>
+      <t>is not provided, the default value will be "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>password</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,14 +185,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -183,6 +195,28 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -212,14 +246,14 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -538,7 +572,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G2" sqref="G2:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,20 +585,20 @@
     <col min="10" max="10" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -584,12 +618,12 @@
       <c r="E2">
         <v>123456</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="G2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -601,47 +635,47 @@
       <c r="E3">
         <v>123456</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>

</xml_diff>